<commit_message>
creacion de linea base 2016
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Linea Base/Plan_Métricas_2016.xlsx
+++ b/Proyectos/2016/Linea Base/Plan_Métricas_2016.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Objetivos de Medición" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="139">
   <si>
     <t>Objetivos de Medición</t>
   </si>
@@ -34,7 +34,7 @@
     <t>Métricas</t>
   </si>
   <si>
-    <t>Tener una desviación miníma del - 15% en esfuerzo y costo de los servicios ofertados con el fin de asegurar la rentabilidad del negocio.</t>
+    <t>Tener una desviación miníma del - 15% en esfuerzo(proyectos generados) y costo de los servicios ofertados con el fin de asegurar la rentabilidad del negocio.</t>
   </si>
   <si>
     <t>Desviación de esfuerzo</t>
@@ -148,7 +148,7 @@
     <t>Mecanismo de Recolección y Almacenamiento</t>
   </si>
   <si>
-    <t>Ingresar al plan de proyecto en la sección estimación y tomar el valor total de los proyectos esperados anualmente y dividirlo entre los doce meses, almacenar dicho dato como esfuerzo planeado, adicional ir al sistema sos soft el cual tiene la cantidad de proyectos registrados y generar la sumatoria de los registros en color rojo, generar el calculo especificado previamente y almacenarlo en el concentrado de métricas en la pestaña esfuerzo</t>
+    <t>Ingresar al plan de proyecto en la sección estimación y tomar el valor total de los proyectos esperados anualmente y dividirlo entre los doce meses, almacenar dicho dato como esfuerzo planeado, adicional ir al documento control de ventas el cual tiene la cantidad de proyectos registrados y generar la sumatoria de los registros en que pertenezcan a la fecha de evaluacion, dicho resultado solo pertenece a la seccion de ventas, para obtener la sección de soporte se deberá ingresar a bitrix en la pestaña CRM, Activities ,presionar el botón mas y poner iniciales de persona a filtrar,  presionar el cuadro posicionado a la derecha del botón mas e ingresar nombre de persona y tareas completas (se puede filtrar por deadline), generar el calculo especificado previamente y almacenarlo en el concentrado de métricas en la pestaña esfuerzo</t>
   </si>
   <si>
     <t>Periodicidad</t>
@@ -178,18 +178,7 @@
     <t>A quien se presenta el reporte de métricas</t>
   </si>
   <si>
-    <r>
-      <t>Guía de análisis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
+    <t>Guía de análisis: </t>
   </si>
   <si>
     <t>El análisis se hara en base a la grafica de Desviación</t>
@@ -384,20 +373,6 @@
     <t>A quien se le presenta el reporte de métricas</t>
   </si>
   <si>
-    <r>
-      <t>Guía de análisis:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t> </t>
-    </r>
-  </si>
-  <si>
     <t>Que el índice de crecimiento en ventas sea mayor o igual a 40% </t>
   </si>
   <si>
@@ -474,10 +449,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00;[RED]\$#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="\$#,##0.00;[RED]\$#,##0.00"/>
   </numFmts>
   <fonts count="17">
     <font>
@@ -551,6 +527,7 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -656,10 +633,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -690,7 +667,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -803,6 +780,10 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -896,6 +877,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1003,7 +988,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1320,11 +1305,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="44456943"/>
-        <c:axId val="37986921"/>
+        <c:axId val="30562196"/>
+        <c:axId val="54346513"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44456943"/>
+        <c:axId val="30562196"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1341,14 +1326,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="37986921"/>
+        <c:crossAx val="54346513"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="37986921"/>
+        <c:axId val="54346513"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1398,7 +1383,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44456943"/>
+        <c:crossAx val="30562196"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1428,7 +1413,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1442,17 +1427,19 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$AB$38</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AB$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Costo planeado</c:v>
+                  <c:v>Esfuerzo planeado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="4f81bd"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1467,7 +1454,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$AA$39:$AA$47</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AA$39:$AA$47</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1502,24 +1489,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de costos'!$AB$39:$AB$47</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AB$39:$AB$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>3287</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5344</c:v>
+                  <c:v>234</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3423</c:v>
+                  <c:v>543</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>40000</c:v>
+                  <c:v>342</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5467</c:v>
+                  <c:v>344</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>532</c:v>
@@ -1528,7 +1515,7 @@
                   <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>900</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>324</c:v>
@@ -1542,17 +1529,19 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$AC$38</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AC$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Costo real</c:v>
+                  <c:v>Esfuerzo real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="c0504d"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1567,7 +1556,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$AA$39:$AA$47</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AA$39:$AA$47</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1602,24 +1591,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de costos'!$AC$39:$AC$47</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AC$39:$AC$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4076</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4088</c:v>
+                  <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5076</c:v>
+                  <c:v>343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37000</c:v>
+                  <c:v>331</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4980</c:v>
+                  <c:v>434</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>533</c:v>
@@ -1628,7 +1617,7 @@
                   <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1500</c:v>
+                  <c:v>33</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>342</c:v>
@@ -1642,17 +1631,19 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$AD$38</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AD$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Desviacion del costo</c:v>
+                  <c:v>Desviacion de esfuerzo %</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:noFill/>
+            <a:solidFill>
+              <a:srgbClr val="9bbb59"/>
+            </a:solidFill>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1667,7 +1658,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Desviacion de costos'!$AA$39:$AA$47</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AA$39:$AA$47</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -1702,36 +1693,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de costos'!$AD$39:$AD$47</c:f>
+              <c:f>'Desviacion de esfuerzo'!$AD$39:$AD$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>789</c:v>
+                  <c:v>-0.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1256</c:v>
+                  <c:v>-1.81</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1653</c:v>
+                  <c:v>-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-3000</c:v>
+                  <c:v>-0.11</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-487</c:v>
+                  <c:v>0.9</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>600</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>18</c:v>
+                  <c:v>0.18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1739,11 +1730,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="24000606"/>
-        <c:axId val="88253382"/>
+        <c:axId val="41599120"/>
+        <c:axId val="9022554"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="24000606"/>
+        <c:axId val="41599120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1760,14 +1751,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="88253382"/>
+        <c:crossAx val="9022554"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="88253382"/>
+        <c:axId val="9022554"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1817,7 +1808,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="24000606"/>
+        <c:crossAx val="41599120"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1847,7 +1838,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2164,11 +2155,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="3118801"/>
-        <c:axId val="35554754"/>
+        <c:axId val="77456780"/>
+        <c:axId val="35198731"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="3118801"/>
+        <c:axId val="77456780"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2185,14 +2176,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="35554754"/>
+        <c:crossAx val="35198731"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="35554754"/>
+        <c:axId val="35198731"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2242,7 +2233,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="3118801"/>
+        <c:crossAx val="77456780"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2272,7 +2263,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2589,11 +2580,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="14317685"/>
-        <c:axId val="80842333"/>
+        <c:axId val="77086402"/>
+        <c:axId val="77474356"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="14317685"/>
+        <c:axId val="77086402"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2610,14 +2601,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="80842333"/>
+        <c:crossAx val="77474356"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="80842333"/>
+        <c:axId val="77474356"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2667,7 +2658,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="14317685"/>
+        <c:crossAx val="77086402"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -2697,7 +2688,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2711,19 +2702,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de esfuerzo'!$AB$38</c:f>
+              <c:f>'Desviacion de costos'!$AB$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Esfuerzo planeado</c:v>
+                  <c:v>Costo planeado</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="4f81bd"/>
-            </a:solidFill>
+            <a:noFill/>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2738,7 +2727,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Desviacion de esfuerzo'!$AA$39:$AA$47</c:f>
+              <c:f>'Desviacion de costos'!$AA$39:$AA$47</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2773,24 +2762,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$AB$39:$AB$47</c:f>
+              <c:f>'Desviacion de costos'!$AB$39:$AB$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>3287</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>234</c:v>
+                  <c:v>5344</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>543</c:v>
+                  <c:v>3423</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>342</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>344</c:v>
+                  <c:v>5467</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>532</c:v>
@@ -2799,7 +2788,7 @@
                   <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>23</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>324</c:v>
@@ -2813,19 +2802,17 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de esfuerzo'!$AC$38</c:f>
+              <c:f>'Desviacion de costos'!$AC$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Esfuerzo real</c:v>
+                  <c:v>Costo real</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="c0504d"/>
-            </a:solidFill>
+            <a:noFill/>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2840,7 +2827,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Desviacion de esfuerzo'!$AA$39:$AA$47</c:f>
+              <c:f>'Desviacion de costos'!$AA$39:$AA$47</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2875,24 +2862,24 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$AC$39:$AC$47</c:f>
+              <c:f>'Desviacion de costos'!$AC$39:$AC$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>80</c:v>
+                  <c:v>4076</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>53</c:v>
+                  <c:v>4088</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>343</c:v>
+                  <c:v>5076</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>331</c:v>
+                  <c:v>37000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>434</c:v>
+                  <c:v>4980</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>533</c:v>
@@ -2901,7 +2888,7 @@
                   <c:v>534</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>33</c:v>
+                  <c:v>1500</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>342</c:v>
@@ -2915,19 +2902,17 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Desviacion de esfuerzo'!$AD$38</c:f>
+              <c:f>'Desviacion de costos'!$AD$38</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Desviacion de esfuerzo %</c:v>
+                  <c:v>Desviacion del costo</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="9bbb59"/>
-            </a:solidFill>
+            <a:noFill/>
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -2942,7 +2927,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>'Desviacion de esfuerzo'!$AA$39:$AA$47</c:f>
+              <c:f>'Desviacion de costos'!$AA$39:$AA$47</c:f>
               <c:strCache>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
@@ -2977,36 +2962,36 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Desviacion de esfuerzo'!$AD$39:$AD$47</c:f>
+              <c:f>'Desviacion de costos'!$AD$39:$AD$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>-0.2</c:v>
+                  <c:v>789</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-1.81</c:v>
+                  <c:v>-1256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2</c:v>
+                  <c:v>1653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-0.11</c:v>
+                  <c:v>-3000</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.9</c:v>
+                  <c:v>-487</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.01</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.1</c:v>
+                  <c:v>600</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.18</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3014,11 +2999,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="29238868"/>
-        <c:axId val="34303961"/>
+        <c:axId val="80275608"/>
+        <c:axId val="24511347"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="29238868"/>
+        <c:axId val="80275608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3035,14 +3020,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="34303961"/>
+        <c:crossAx val="24511347"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="34303961"/>
+        <c:axId val="24511347"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3092,7 +3077,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="29238868"/>
+        <c:crossAx val="80275608"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3122,7 +3107,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -3439,11 +3424,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="79945680"/>
-        <c:axId val="10903799"/>
+        <c:axId val="13841932"/>
+        <c:axId val="13891094"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="79945680"/>
+        <c:axId val="13841932"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3460,14 +3445,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="10903799"/>
+        <c:crossAx val="13891094"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="10903799"/>
+        <c:axId val="13891094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3517,7 +3502,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="79945680"/>
+        <c:crossAx val="13841932"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -3552,15 +3537,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>144720</xdr:rowOff>
+      <xdr:rowOff>117720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>170280</xdr:rowOff>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3568,8 +3553,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="44032320" y="9348120"/>
-        <a:ext cx="5979600" cy="2883240"/>
+        <a:off x="43399800" y="10180440"/>
+        <a:ext cx="5860080" cy="2882160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3582,15 +3567,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>270360</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>129960</xdr:rowOff>
+      <xdr:rowOff>102960</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3258720</xdr:colOff>
+      <xdr:colOff>3339000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2051640</xdr:rowOff>
+      <xdr:rowOff>2023920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3603,8 +3588,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392040" y="698760"/>
-          <a:ext cx="5978520" cy="2112120"/>
+          <a:off x="461880" y="671760"/>
+          <a:ext cx="5937480" cy="2111400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3619,15 +3604,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3446640</xdr:colOff>
+      <xdr:colOff>3528000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>187200</xdr:rowOff>
+      <xdr:rowOff>160200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>7425720</xdr:colOff>
+      <xdr:colOff>7506000</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2007360</xdr:rowOff>
+      <xdr:rowOff>1979640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3640,8 +3625,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6558480" y="756000"/>
-          <a:ext cx="3979080" cy="2010600"/>
+          <a:off x="6588360" y="729000"/>
+          <a:ext cx="3978000" cy="2009880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3661,15 +3646,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>32</xdr:col>
-      <xdr:colOff>366840</xdr:colOff>
+      <xdr:colOff>447840</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>50040</xdr:rowOff>
+      <xdr:rowOff>23040</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>40</xdr:col>
-      <xdr:colOff>338760</xdr:colOff>
+      <xdr:colOff>418680</xdr:colOff>
       <xdr:row>49</xdr:row>
-      <xdr:rowOff>162000</xdr:rowOff>
+      <xdr:rowOff>133920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3677,8 +3662,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="43219080" y="9854280"/>
-        <a:ext cx="8100000" cy="3350520"/>
+        <a:off x="42580080" y="9827280"/>
+        <a:ext cx="7941240" cy="3349440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3691,15 +3676,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>317880</xdr:rowOff>
+      <xdr:rowOff>290880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2167560</xdr:colOff>
+      <xdr:colOff>2247480</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2202480</xdr:rowOff>
+      <xdr:rowOff>2174400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3712,8 +3697,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392040" y="889200"/>
-          <a:ext cx="4887360" cy="2435040"/>
+          <a:off x="461520" y="862200"/>
+          <a:ext cx="4846320" cy="2433960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3728,15 +3713,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2189160</xdr:colOff>
+      <xdr:colOff>2270160</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>289440</xdr:rowOff>
+      <xdr:rowOff>262440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>205560</xdr:colOff>
+      <xdr:colOff>285480</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2190960</xdr:rowOff>
+      <xdr:rowOff>2162880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3749,8 +3734,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5301000" y="860760"/>
-          <a:ext cx="5968080" cy="2451960"/>
+          <a:off x="5330520" y="833760"/>
+          <a:ext cx="5877360" cy="2450880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3770,15 +3755,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>78840</xdr:rowOff>
+      <xdr:rowOff>51840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>77040</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3786,8 +3771,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="45531720" y="9071640"/>
-        <a:ext cx="5979240" cy="2883600"/>
+        <a:off x="44875440" y="9044640"/>
+        <a:ext cx="5860080" cy="2882520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3800,15 +3785,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>128880</xdr:rowOff>
+      <xdr:rowOff>101880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4037760</xdr:colOff>
+      <xdr:colOff>4117680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2307600</xdr:rowOff>
+      <xdr:rowOff>2279520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3821,8 +3806,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392040" y="736920"/>
-          <a:ext cx="6757560" cy="2369160"/>
+          <a:off x="461520" y="709920"/>
+          <a:ext cx="6716520" cy="2368080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3837,15 +3822,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>4703760</xdr:colOff>
+      <xdr:colOff>4784760</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>43200</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>8501760</xdr:colOff>
+      <xdr:colOff>8581680</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2285280</xdr:rowOff>
+      <xdr:rowOff>2257200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3858,8 +3843,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7815600" y="651240"/>
-          <a:ext cx="3798000" cy="2432520"/>
+          <a:off x="7845120" y="624240"/>
+          <a:ext cx="3796920" cy="2431440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3879,15 +3864,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3895,8 +3880,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42571800" y="9290880"/>
-        <a:ext cx="5979600" cy="2883240"/>
+        <a:off x="41946840" y="9263880"/>
+        <a:ext cx="5860080" cy="2882160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3909,15 +3894,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2194200</xdr:colOff>
+      <xdr:colOff>2274120</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2344320</xdr:rowOff>
+      <xdr:rowOff>2316240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3930,8 +3915,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="392040" y="889200"/>
-          <a:ext cx="4914000" cy="2407320"/>
+          <a:off x="461520" y="862200"/>
+          <a:ext cx="4872960" cy="2406240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3946,15 +3931,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2220120</xdr:colOff>
+      <xdr:colOff>2301120</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>108360</xdr:rowOff>
+      <xdr:rowOff>81360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>6368040</xdr:colOff>
+      <xdr:colOff>6447960</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2359080</xdr:rowOff>
+      <xdr:rowOff>2331000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -3967,8 +3952,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5331960" y="870120"/>
-          <a:ext cx="4147920" cy="2441160"/>
+          <a:off x="5361480" y="843120"/>
+          <a:ext cx="4146840" cy="2440080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -3988,15 +3973,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>77760</xdr:rowOff>
+      <xdr:rowOff>50760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>103680</xdr:rowOff>
+      <xdr:rowOff>75600</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4004,8 +3989,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42089400" y="9212760"/>
-        <a:ext cx="5979240" cy="2883240"/>
+        <a:off x="41466600" y="9185760"/>
+        <a:ext cx="5860440" cy="2882160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4018,15 +4003,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>979560</xdr:colOff>
+      <xdr:colOff>1060560</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2586600</xdr:colOff>
+      <xdr:colOff>2666520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2365200</xdr:rowOff>
+      <xdr:rowOff>2337120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4039,8 +4024,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1182600" y="698760"/>
-          <a:ext cx="4515840" cy="2428200"/>
+          <a:off x="1252080" y="671760"/>
+          <a:ext cx="4474800" cy="2427120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4060,15 +4045,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>417600</xdr:colOff>
+      <xdr:colOff>498600</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>79200</xdr:rowOff>
+      <xdr:rowOff>52200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>300960</xdr:colOff>
+      <xdr:colOff>380880</xdr:colOff>
       <xdr:row>48</xdr:row>
-      <xdr:rowOff>104760</xdr:rowOff>
+      <xdr:rowOff>76680</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4076,8 +4061,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42368760" y="9127080"/>
-        <a:ext cx="5979240" cy="2883240"/>
+        <a:off x="41742360" y="9100080"/>
+        <a:ext cx="5860080" cy="2882160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4090,15 +4075,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>636840</xdr:colOff>
+      <xdr:colOff>717840</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>155880</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2063160</xdr:colOff>
+      <xdr:colOff>2143080</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2280960</xdr:rowOff>
+      <xdr:rowOff>2252880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4111,8 +4096,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="839880" y="727200"/>
-          <a:ext cx="4335120" cy="2315520"/>
+          <a:off x="909360" y="700200"/>
+          <a:ext cx="4294080" cy="2314440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4132,15 +4117,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1007640</xdr:colOff>
+      <xdr:colOff>1088640</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>41760</xdr:rowOff>
+      <xdr:rowOff>14760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>4300920</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>304200</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1706400</xdr:rowOff>
+      <xdr:rowOff>1678320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4153,8 +4138,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1007640" y="803520"/>
-          <a:ext cx="3293280" cy="1664640"/>
+          <a:off x="1088640" y="776520"/>
+          <a:ext cx="4353120" cy="1663560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4169,15 +4154,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1692000</xdr:colOff>
+      <xdr:colOff>1773000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>184680</xdr:rowOff>
+      <xdr:rowOff>157680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>5280480</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>55080</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1771560</xdr:rowOff>
+      <xdr:rowOff>1743480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4190,8 +4175,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6886800" y="756000"/>
-          <a:ext cx="3588480" cy="1777320"/>
+          <a:off x="6910560" y="729000"/>
+          <a:ext cx="4968000" cy="1776240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4211,15 +4196,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>189000</xdr:colOff>
+      <xdr:colOff>270000</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>127440</xdr:rowOff>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>538920</xdr:colOff>
+      <xdr:colOff>618840</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2150280</xdr:rowOff>
+      <xdr:rowOff>2122200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4232,8 +4217,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="189000" y="870120"/>
-          <a:ext cx="4490640" cy="2213280"/>
+          <a:off x="270000" y="843120"/>
+          <a:ext cx="4442040" cy="2212200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4256,17 +4241,17 @@
   <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.71255060728745"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.7125506072875"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="45.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="2.56275303643725"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="47.1093117408907"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="44.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.4372469635628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.7692307692308"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4296,7 +4281,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B4" s="5"/>
       <c r="C4" s="6" t="s">
         <v>5</v>
@@ -4460,20 +4445,20 @@
   </sheetPr>
   <dimension ref="1:47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B22" activeCellId="0" sqref="B22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="109.425101214575"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="108.267206477733"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15795,7 +15780,7 @@
       <c r="AMI11" s="0"/>
       <c r="AMJ11" s="0"/>
     </row>
-    <row r="12" customFormat="false" ht="48" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+    <row r="12" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="27" t="s">
         <v>40</v>
@@ -24033,10 +24018,10 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A20" s="0"/>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="D20" s="0"/>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
@@ -25059,17 +25044,17 @@
       <c r="AMI20" s="0"/>
       <c r="AMJ20" s="0"/>
     </row>
-    <row r="21" s="28" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B21" s="29" t="s">
+    <row r="21" s="29" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
+      <c r="B21" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="C21" s="29"/>
+      <c r="C21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C22" s="32" t="s">
         <v>53</v>
       </c>
       <c r="AA22" s="0"/>
@@ -25078,7 +25063,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="33" t="s">
         <v>54</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -25090,7 +25075,7 @@
       <c r="AD23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="34" t="s">
         <v>56</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -25203,7 +25188,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -25218,7 +25203,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -25233,7 +25218,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -25248,7 +25233,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -25263,7 +25248,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -25278,7 +25263,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -25293,7 +25278,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -25308,7 +25293,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -25323,7 +25308,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -25359,19 +25344,19 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="89.421052631579"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="88.417004048583"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -25588,20 +25573,20 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="31" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>53</v>
       </c>
       <c r="AA21" s="0"/>
@@ -25610,7 +25595,7 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>54</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -25622,7 +25607,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="33" t="s">
+      <c r="B23" s="34" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="8" t="s">
@@ -25735,13 +25720,13 @@
       <c r="AA39" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="AB39" s="35" t="n">
+      <c r="AB39" s="36" t="n">
         <v>3287</v>
       </c>
-      <c r="AC39" s="35" t="n">
+      <c r="AC39" s="36" t="n">
         <v>4076</v>
       </c>
-      <c r="AD39" s="36" t="n">
+      <c r="AD39" s="37" t="n">
         <f aca="false">(AC39-AB39)</f>
         <v>789</v>
       </c>
@@ -25750,13 +25735,13 @@
       <c r="AA40" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="AB40" s="35" t="n">
+      <c r="AB40" s="36" t="n">
         <v>5344</v>
       </c>
-      <c r="AC40" s="35" t="n">
+      <c r="AC40" s="36" t="n">
         <v>4088</v>
       </c>
-      <c r="AD40" s="36" t="n">
+      <c r="AD40" s="37" t="n">
         <f aca="false">(AC40-AB40)</f>
         <v>-1256</v>
       </c>
@@ -25765,13 +25750,13 @@
       <c r="AA41" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AB41" s="35" t="n">
+      <c r="AB41" s="36" t="n">
         <v>3423</v>
       </c>
-      <c r="AC41" s="35" t="n">
+      <c r="AC41" s="36" t="n">
         <v>5076</v>
       </c>
-      <c r="AD41" s="36" t="n">
+      <c r="AD41" s="37" t="n">
         <f aca="false">(AC41-AB41)</f>
         <v>1653</v>
       </c>
@@ -25780,13 +25765,13 @@
       <c r="AA42" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="AB42" s="35" t="n">
+      <c r="AB42" s="36" t="n">
         <v>40000</v>
       </c>
-      <c r="AC42" s="35" t="n">
+      <c r="AC42" s="36" t="n">
         <v>37000</v>
       </c>
-      <c r="AD42" s="36" t="n">
+      <c r="AD42" s="37" t="n">
         <f aca="false">(AC42-AB42)</f>
         <v>-3000</v>
       </c>
@@ -25795,13 +25780,13 @@
       <c r="AA43" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="AB43" s="35" t="n">
+      <c r="AB43" s="36" t="n">
         <v>5467</v>
       </c>
-      <c r="AC43" s="35" t="n">
+      <c r="AC43" s="36" t="n">
         <v>4980</v>
       </c>
-      <c r="AD43" s="36" t="n">
+      <c r="AD43" s="37" t="n">
         <f aca="false">(AC43-AB43)</f>
         <v>-487</v>
       </c>
@@ -25810,13 +25795,13 @@
       <c r="AA44" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="AB44" s="35" t="n">
+      <c r="AB44" s="36" t="n">
         <v>532</v>
       </c>
-      <c r="AC44" s="35" t="n">
+      <c r="AC44" s="36" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="36" t="n">
+      <c r="AD44" s="37" t="n">
         <f aca="false">(AC44-AB44)</f>
         <v>1</v>
       </c>
@@ -25825,13 +25810,13 @@
       <c r="AA45" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="AB45" s="35" t="n">
+      <c r="AB45" s="36" t="n">
         <v>534</v>
       </c>
-      <c r="AC45" s="35" t="n">
+      <c r="AC45" s="36" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="36" t="n">
+      <c r="AD45" s="37" t="n">
         <f aca="false">(AC45-AB45)</f>
         <v>0</v>
       </c>
@@ -25840,13 +25825,13 @@
       <c r="AA46" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="AB46" s="35" t="n">
+      <c r="AB46" s="36" t="n">
         <v>900</v>
       </c>
-      <c r="AC46" s="35" t="n">
+      <c r="AC46" s="36" t="n">
         <v>1500</v>
       </c>
-      <c r="AD46" s="36" t="n">
+      <c r="AD46" s="37" t="n">
         <f aca="false">(AC46-AB46)</f>
         <v>600</v>
       </c>
@@ -25855,13 +25840,13 @@
       <c r="AA47" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="AB47" s="35" t="n">
+      <c r="AB47" s="36" t="n">
         <v>324</v>
       </c>
-      <c r="AC47" s="35" t="n">
+      <c r="AC47" s="36" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="36" t="n">
+      <c r="AD47" s="37" t="n">
         <f aca="false">(AC47-AB47)</f>
         <v>18</v>
       </c>
@@ -25901,18 +25886,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="126.287449392713"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="124.866396761134"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -26123,20 +26108,20 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="39" t="s">
+      <c r="C21" s="40" t="s">
         <v>86</v>
       </c>
       <c r="AA21" s="0"/>
@@ -26145,7 +26130,7 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -26157,7 +26142,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -26276,7 +26261,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -26291,7 +26276,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -26306,7 +26291,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -26321,7 +26306,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -26336,7 +26321,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -26351,7 +26336,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -26366,7 +26351,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -26381,7 +26366,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -26396,7 +26381,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -26436,18 +26421,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="93"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="91.9311740890688"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -26527,7 +26512,7 @@
       <c r="B8" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="C8" s="42" t="s">
+      <c r="C8" s="43" t="s">
         <v>93</v>
       </c>
       <c r="AA8" s="0"/>
@@ -26539,7 +26524,7 @@
       <c r="B9" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="42"/>
+      <c r="C9" s="43"/>
       <c r="AA9" s="0"/>
       <c r="AB9" s="0"/>
       <c r="AC9" s="0"/>
@@ -26549,7 +26534,7 @@
       <c r="B10" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="C10" s="42"/>
+      <c r="C10" s="43"/>
       <c r="AA10" s="0"/>
       <c r="AB10" s="0"/>
       <c r="AC10" s="0"/>
@@ -26658,20 +26643,20 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>86</v>
       </c>
       <c r="AA21" s="0"/>
@@ -26680,7 +26665,7 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -26692,7 +26677,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -26811,7 +26796,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -26826,7 +26811,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -26841,7 +26826,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -26856,7 +26841,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -26871,7 +26856,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -26886,7 +26871,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -26901,7 +26886,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -26916,7 +26901,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -26931,7 +26916,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -26971,18 +26956,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="87.5748987854251"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="86.5303643724696"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -27193,20 +27178,20 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>86</v>
       </c>
       <c r="AA21" s="0"/>
@@ -27215,7 +27200,7 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -27227,7 +27212,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -27346,7 +27331,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -27361,7 +27346,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -27376,7 +27361,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -27391,7 +27376,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -27406,7 +27391,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -27421,7 +27406,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -27436,7 +27421,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -27451,7 +27436,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -27466,7 +27451,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -27506,18 +27491,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.2834008097166"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.7125506072874"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="90.7165991902834"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.7085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="25"/>
-    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.4251012145749"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.7125506072875"/>
-    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="22" width="2.15789473684211"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="22" width="32.2631578947368"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="22" width="89.6315789473684"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="22" width="18.4939271255061"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="22" width="24.7004048582996"/>
+    <col collapsed="false" hidden="false" max="27" min="6" style="22" width="11.2064777327935"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="22" width="16.4696356275304"/>
+    <col collapsed="false" hidden="false" max="1025" min="29" style="22" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="14" t="str">
@@ -27728,20 +27713,20 @@
       <c r="AD19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="C20" s="14"/>
+      <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
       <c r="AB20" s="0"/>
       <c r="AC20" s="0"/>
       <c r="AD20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
-      <c r="B21" s="43" t="s">
+      <c r="B21" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="31" t="s">
+      <c r="C21" s="32" t="s">
         <v>86</v>
       </c>
       <c r="AA21" s="0"/>
@@ -27750,7 +27735,7 @@
       <c r="AD21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="41" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="6" t="s">
@@ -27762,7 +27747,7 @@
       <c r="AD22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>89</v>
       </c>
       <c r="C23" s="6" t="s">
@@ -27881,7 +27866,7 @@
       <c r="AC39" s="22" t="n">
         <v>80</v>
       </c>
-      <c r="AD39" s="34" t="n">
+      <c r="AD39" s="35" t="n">
         <f aca="false">(AC39-AB39)/100</f>
         <v>-0.2</v>
       </c>
@@ -27896,7 +27881,7 @@
       <c r="AC40" s="22" t="n">
         <v>53</v>
       </c>
-      <c r="AD40" s="34" t="n">
+      <c r="AD40" s="35" t="n">
         <f aca="false">(AC40-AB40)/100</f>
         <v>-1.81</v>
       </c>
@@ -27911,7 +27896,7 @@
       <c r="AC41" s="22" t="n">
         <v>343</v>
       </c>
-      <c r="AD41" s="34" t="n">
+      <c r="AD41" s="35" t="n">
         <f aca="false">(AC41-AB41)/100</f>
         <v>-2</v>
       </c>
@@ -27926,7 +27911,7 @@
       <c r="AC42" s="22" t="n">
         <v>331</v>
       </c>
-      <c r="AD42" s="34" t="n">
+      <c r="AD42" s="35" t="n">
         <f aca="false">(AC42-AB42)/100</f>
         <v>-0.11</v>
       </c>
@@ -27941,7 +27926,7 @@
       <c r="AC43" s="22" t="n">
         <v>434</v>
       </c>
-      <c r="AD43" s="34" t="n">
+      <c r="AD43" s="35" t="n">
         <f aca="false">(AC43-AB43)/100</f>
         <v>0.9</v>
       </c>
@@ -27956,7 +27941,7 @@
       <c r="AC44" s="22" t="n">
         <v>533</v>
       </c>
-      <c r="AD44" s="34" t="n">
+      <c r="AD44" s="35" t="n">
         <f aca="false">(AC44-AB44)/100</f>
         <v>0.01</v>
       </c>
@@ -27971,7 +27956,7 @@
       <c r="AC45" s="22" t="n">
         <v>534</v>
       </c>
-      <c r="AD45" s="34" t="n">
+      <c r="AD45" s="35" t="n">
         <f aca="false">(AC45-AB45)/100</f>
         <v>0</v>
       </c>
@@ -27986,7 +27971,7 @@
       <c r="AC46" s="22" t="n">
         <v>33</v>
       </c>
-      <c r="AD46" s="34" t="n">
+      <c r="AD46" s="35" t="n">
         <f aca="false">(AC46-AB46)/100</f>
         <v>0.1</v>
       </c>
@@ -28001,7 +27986,7 @@
       <c r="AC47" s="22" t="n">
         <v>342</v>
       </c>
-      <c r="AD47" s="34" t="n">
+      <c r="AD47" s="35" t="n">
         <f aca="false">(AC47-AB47)/100</f>
         <v>0.18</v>
       </c>
@@ -28041,96 +28026,96 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="58.421052631579"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.9959514170041"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.5748987854251"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="57.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="75.1902834008097"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="10.3886639676113"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="46" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="44" t="s">
+      <c r="A2" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="44" t="s">
+      <c r="A3" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="47" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="s">
+      <c r="A4" s="48" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="47"/>
+      <c r="B4" s="48"/>
     </row>
     <row r="5" customFormat="false" ht="141" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48"/>
-      <c r="B5" s="48"/>
+      <c r="A5" s="49"/>
+      <c r="B5" s="49"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
+      <c r="A6" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="47"/>
+      <c r="B6" s="48"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
+      <c r="A7" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="47" t="s">
+      <c r="B7" s="48" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="49" t="s">
+      <c r="A8" s="50" t="s">
         <v>107</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="51" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="B9" s="50"/>
+      <c r="B9" s="51"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B10" s="50"/>
+      <c r="B10" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B11" s="47"/>
+      <c r="B11" s="48"/>
     </row>
     <row r="12" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="51" t="s">
+      <c r="A12" s="52" t="s">
         <v>111</v>
       </c>
-      <c r="B12" s="51"/>
+      <c r="B12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="47" t="s">
+      <c r="B13" s="48" t="s">
         <v>42</v>
       </c>
     </row>
@@ -28143,16 +28128,16 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47" t="s">
+      <c r="A15" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="47"/>
+      <c r="B15" s="48"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="48" t="s">
         <v>46</v>
       </c>
     </row>
@@ -28165,10 +28150,10 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="B18" s="47" t="s">
+      <c r="B18" s="48" t="s">
         <v>114</v>
       </c>
     </row>
@@ -28181,33 +28166,33 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B20" s="53"/>
+    </row>
+    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="B20" s="47"/>
-    </row>
-    <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="52" t="s">
+      <c r="B21" s="27" t="s">
         <v>116</v>
       </c>
-      <c r="B21" s="27" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="55" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="53" t="s">
+      <c r="B22" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="B22" s="27" t="s">
+    </row>
+    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="56" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="54" t="s">
+      <c r="B23" s="27" t="s">
         <v>120</v>
-      </c>
-      <c r="B23" s="27" t="s">
-        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -28239,82 +28224,82 @@
   </sheetPr>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.5668016194332"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="59.1457489878543"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.4251012145749"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="46.0323886639676"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.4493927125506"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.2064777327935"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="55" t="str">
+      <c r="B1" s="57" t="str">
         <f aca="false">'Objetivos de Medición'!C9</f>
         <v>Índice de Satisfacción</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="58" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="47" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="58" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="56" t="s">
-        <v>69</v>
-      </c>
-      <c r="B3" s="46" t="s">
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="59" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="59"/>
+    </row>
+    <row r="5" customFormat="false" ht="184.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="60"/>
+      <c r="B5" s="60"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="48"/>
+      <c r="Q6" s="0" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="57" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" s="57"/>
-    </row>
-    <row r="5" customFormat="false" ht="184.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58"/>
-      <c r="B5" s="58"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" s="47"/>
-      <c r="Q6" s="0" t="s">
+      <c r="R6" s="0" t="s">
         <v>124</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="S6" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="T6" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="T6" s="0" t="s">
+      <c r="U6" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="U6" s="0" t="s">
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="P7" s="0" t="s">
         <v>128</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="P7" s="0" t="s">
-        <v>129</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">AVERAGE(R7:U7)</f>
@@ -28335,13 +28320,13 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="B8" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="P8" s="0" t="s">
         <v>131</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>132</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">AVERAGE(R8:U8)</f>
@@ -28361,22 +28346,22 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="s">
+      <c r="A9" s="48" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="47"/>
+      <c r="B9" s="48"/>
     </row>
     <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="51" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="51"/>
+      <c r="A10" s="52" t="s">
+        <v>132</v>
+      </c>
+      <c r="B10" s="52"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="48" t="s">
         <v>41</v>
       </c>
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="48" t="s">
         <v>42</v>
       </c>
     </row>
@@ -28389,16 +28374,16 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="47"/>
+      <c r="B13" s="48"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="48" t="s">
         <v>46</v>
       </c>
     </row>
@@ -28411,10 +28396,10 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="48" t="s">
         <v>114</v>
       </c>
     </row>
@@ -28427,39 +28412,39 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="47" t="s">
-        <v>115</v>
-      </c>
-      <c r="B18" s="47"/>
+      <c r="A18" s="53" t="s">
+        <v>50</v>
+      </c>
+      <c r="B18" s="53"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="59" t="s">
+      <c r="A19" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="B19" s="61"/>
+    </row>
+    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="54" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="59"/>
-    </row>
-    <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="52" t="s">
+      <c r="B20" s="27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="55" t="s">
         <v>135</v>
       </c>
-      <c r="B20" s="27" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="53" t="s">
+      <c r="B21" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="B21" s="27" t="s">
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="56" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="54" t="s">
+      <c r="B22" s="27" t="s">
         <v>138</v>
-      </c>
-      <c r="B22" s="27" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se apoyo a ricardo para actualizar las formulas y de resultados para que se visualizaran en porcentaje
</commit_message>
<xml_diff>
--- a/Proyectos/2016/Linea Base/Plan_Métricas_2016.xlsx
+++ b/Proyectos/2016/Linea Base/Plan_Métricas_2016.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="485" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="483" uniqueCount="167">
   <si>
     <t>Objetivos de Medición</t>
   </si>
@@ -147,16 +147,13 @@
     <t>Esfuerzo planeado</t>
   </si>
   <si>
-    <t>Desviación de Esfuerzo (#tickets)  = Esfuerzo real – Esfuerzo planeado</t>
+    <t>Desviación(%)= ((Esfuerzo real)/Esfuerzo planeado)-1</t>
   </si>
   <si>
     <t>Esfuerzo real</t>
   </si>
   <si>
     <t>Desviación</t>
-  </si>
-  <si>
-    <t>Desviación(%)= ((Esfuerzo real * 100)/Esfuerzo planeado)-100</t>
   </si>
   <si>
     <t>Mecanismo de Recolección y Almacenamiento</t>
@@ -258,13 +255,10 @@
     <t>Costo planeado</t>
   </si>
   <si>
-    <t>Desviación de Costo($)  = costo planeado – costo real</t>
-  </si>
-  <si>
     <t>Costo real</t>
   </si>
   <si>
-    <t>Desviación(%)= ((Costo planeado * 100)/Costo real)-100</t>
+    <t>Desviación(%)= (Costo planeado/Costo real)-1</t>
   </si>
   <si>
     <t>Tomar el costo estimado en el plan de proyecto dividido entre doce meses como costo planeado y tomar el total gastado entre servicios y sueldos de personal registrados en el mes, dicho dato será otorgado por administración aplicar formula de desviación en porcentaje y plasmar en el concentrado de métricas en la pestaña costos.</t>
@@ -480,7 +474,10 @@
     <t>¿Cual es el producto mas vendido en la empresa?                                             </t>
   </si>
   <si>
-    <t>Productos vendidos=(sumatoria del mes por producto)</t>
+    <t>Sumatoria de productos vendidos</t>
+  </si>
+  <si>
+    <t>Productos vendidos=(sumatoria por producto en el año)</t>
   </si>
   <si>
     <t>Ingresar a bitrix en la pestaña CRM , reportes y ventas por productos, los resultados pasarlos al concentrado de métricas en pestaña productos</t>
@@ -507,7 +504,10 @@
     <t>¿Qué porcentaje de actividades se resolvieron en el tiempo planeado?                                             </t>
   </si>
   <si>
-    <t>Porcentaje de actividades a tiempo =(actividades a tiempo entre actividades a tiempo mas actividades fuera de tiempo)*100</t>
+    <t>Actividades a tiempo, actividades totales</t>
+  </si>
+  <si>
+    <t>Porcentaje de actividades a tiempo =(actividades a tiempo /  total de actividades)</t>
   </si>
   <si>
     <t>Ingresar a bitrix24 en los filtros  de actividades de CRM filtrando las actividades por persona y contabilizar las realizadas antes del deadline y adicional las resueltas fuera del dead line, el valor se deberá almacenar en el concentrado de métrica en pestaña actividades</t>
@@ -535,12 +535,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="0%"/>
     <numFmt numFmtId="166" formatCode="\$#,##0.00;[RED]\$#,##0.00"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -624,12 +625,6 @@
     </font>
     <font>
       <b val="true"/>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -656,11 +651,7 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="13"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
+      <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -948,27 +939,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -980,39 +971,39 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="16" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1088,7 +1079,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart48.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1405,11 +1396,11 @@
         </c:ser>
         <c:gapWidth val="150"/>
         <c:overlap val="0"/>
-        <c:axId val="86010434"/>
-        <c:axId val="96082186"/>
+        <c:axId val="8867842"/>
+        <c:axId val="50847618"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="86010434"/>
+        <c:axId val="8867842"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1426,14 +1417,14 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="96082186"/>
+        <c:crossAx val="50847618"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96082186"/>
+        <c:axId val="50847618"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1483,7 +1474,7 @@
             <a:round/>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="86010434"/>
+        <c:crossAx val="8867842"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:dTable>
@@ -1513,7 +1504,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart49.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1590,11 +1581,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="43104593"/>
-        <c:axId val="93815683"/>
+        <c:axId val="47077094"/>
+        <c:axId val="23877714"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="43104593"/>
+        <c:axId val="47077094"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1610,14 +1601,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="93815683"/>
+        <c:crossAx val="23877714"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="93815683"/>
+        <c:axId val="23877714"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1642,7 +1633,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="43104593"/>
+        <c:crossAx val="47077094"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -1677,7 +1668,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart50.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1928,11 +1919,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="44360639"/>
-        <c:axId val="84556474"/>
+        <c:axId val="44905834"/>
+        <c:axId val="23725214"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="44360639"/>
+        <c:axId val="44905834"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1948,14 +1939,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="84556474"/>
+        <c:crossAx val="23725214"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="84556474"/>
+        <c:axId val="23725214"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1980,7 +1971,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="44360639"/>
+        <c:crossAx val="44905834"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2015,7 +2006,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart51.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -2152,11 +2143,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="54196036"/>
-        <c:axId val="69204355"/>
+        <c:axId val="71312120"/>
+        <c:axId val="10238756"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="54196036"/>
+        <c:axId val="71312120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2172,14 +2163,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="69204355"/>
+        <c:crossAx val="10238756"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69204355"/>
+        <c:axId val="10238756"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2204,7 +2195,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="54196036"/>
+        <c:crossAx val="71312120"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2239,254 +2230,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart52.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>label 0</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>satisfacción</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-          </c:spPr>
-          <c:dLbls>
-            <c:dLblPos val="ctr"/>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-          </c:dLbls>
-          <c:cat>
-            <c:strRef>
-              <c:f>categories</c:f>
-              <c:strCache>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>Enero</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Febrero</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Marzo</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>Abril</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>Mayo</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>Junio</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>Julio</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>Agosto</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>Septiembre</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>Octubre</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>Noviembre</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>Diciembre</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>Total</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>0</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>98.8</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>92.572</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>95.686</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v/>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v/>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:gapWidth val="100"/>
-        <c:overlap val="0"/>
-        <c:axId val="2634417"/>
-        <c:axId val="97761632"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2634417"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="97761632"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="97761632"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln>
-              <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:ln>
-            <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
-            </a:solidFill>
-          </a:ln>
-        </c:spPr>
-        <c:crossAx val="2634417"/>
-        <c:crosses val="autoZero"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
-          </a:solidFill>
-        </a:ln>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </c:spPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:srgbClr val="ffffff"/>
-    </a:solidFill>
-    <a:ln>
-      <a:noFill/>
-    </a:ln>
-  </c:spPr>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart65.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="en-US"/>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Producto mas vendido</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2515,6 +2262,7 @@
             </a:ln>
           </c:spPr>
           <c:dLbls>
+            <c:dLblPos val="ctr"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -2553,11 +2301,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="82911308"/>
-        <c:axId val="82945429"/>
+        <c:axId val="20352754"/>
+        <c:axId val="24505115"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="82911308"/>
+        <c:axId val="20352754"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2573,14 +2321,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82945429"/>
+        <c:crossAx val="24505115"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="82945429"/>
+        <c:axId val="24505115"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2605,7 +2353,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="82911308"/>
+        <c:crossAx val="20352754"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2640,30 +2388,10 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart53.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr sz="1300">
-                <a:latin typeface="Arial"/>
-              </a:rPr>
-              <a:t>Grafico de actividades</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-    </c:title>
     <c:plotArea>
       <c:layout/>
       <c:barChart>
@@ -2678,7 +2406,185 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Enero</c:v>
+                  <c:v>Fila 3</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="004586"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:dLbls>
+            <c:dLblPos val="ctr"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="0"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+          </c:dLbls>
+          <c:cat>
+            <c:strRef>
+              <c:f>categories</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Actividades en tiempo</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Actividades fuera de tiempo</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>0</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:gapWidth val="100"/>
+        <c:overlap val="0"/>
+        <c:axId val="66800833"/>
+        <c:axId val="63652499"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="66800833"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="63652499"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="63652499"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="b3b3b3"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="1" sz="900">
+                    <a:latin typeface="Arial"/>
+                  </a:rPr>
+                  <a:t>Cantidad</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln>
+            <a:solidFill>
+              <a:srgbClr val="b3b3b3"/>
+            </a:solidFill>
+          </a:ln>
+        </c:spPr>
+        <c:crossAx val="66800833"/>
+        <c:crosses val="autoZero"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:solidFill>
+            <a:srgbClr val="b3b3b3"/>
+          </a:solidFill>
+        </a:ln>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </c:spPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:srgbClr val="ffffff"/>
+    </a:solidFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart54.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:lang val="en-US"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>label 0</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v/>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2716,7 +2622,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50</c:v>
+                  <c:v>26.3157894736842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2724,11 +2630,11 @@
         </c:ser>
         <c:gapWidth val="100"/>
         <c:overlap val="0"/>
-        <c:axId val="68728092"/>
-        <c:axId val="72845350"/>
+        <c:axId val="69740366"/>
+        <c:axId val="79553874"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="68728092"/>
+        <c:axId val="69740366"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2744,14 +2650,14 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="72845350"/>
+        <c:crossAx val="79553874"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="72845350"/>
+        <c:axId val="79553874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2766,26 +2672,6 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr sz="900">
-                    <a:latin typeface="Arial"/>
-                  </a:rPr>
-                  <a:t>Porcentaje</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -2796,7 +2682,7 @@
             </a:solidFill>
           </a:ln>
         </c:spPr>
-        <c:crossAx val="68728092"/>
+        <c:crossAx val="69740366"/>
         <c:crosses val="autoZero"/>
       </c:valAx>
       <c:spPr>
@@ -2836,15 +2722,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>31</xdr:col>
-      <xdr:colOff>768600</xdr:colOff>
+      <xdr:colOff>795600</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>152640</xdr:rowOff>
+      <xdr:rowOff>143640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>647280</xdr:colOff>
+      <xdr:colOff>673920</xdr:colOff>
       <xdr:row>47</xdr:row>
-      <xdr:rowOff>173880</xdr:rowOff>
+      <xdr:rowOff>164520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2852,8 +2738,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="42012360" y="9010080"/>
-        <a:ext cx="5856480" cy="2878560"/>
+        <a:off x="42039360" y="9001080"/>
+        <a:ext cx="5856120" cy="2878200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2866,15 +2752,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1480320</xdr:colOff>
+      <xdr:colOff>1507320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>241920</xdr:rowOff>
+      <xdr:rowOff>232920</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>2297520</xdr:colOff>
+      <xdr:colOff>2324160</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2205720</xdr:rowOff>
+      <xdr:rowOff>2196360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2882,8 +2768,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="1671840" y="1003680"/>
-        <a:ext cx="3686040" cy="1963800"/>
+        <a:off x="1698840" y="994680"/>
+        <a:ext cx="3685680" cy="1963440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2901,15 +2787,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>759240</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>786240</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>189000</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>380880</xdr:colOff>
+      <xdr:colOff>407520</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>1584720</xdr:rowOff>
+      <xdr:rowOff>1575360</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2917,8 +2803,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="759240" y="769320"/>
-        <a:ext cx="4759200" cy="1577160"/>
+        <a:off x="786240" y="760320"/>
+        <a:ext cx="4758840" cy="1576800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -2935,16 +2821,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>93600</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>780120</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>186840</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>53280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>656640</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>17280</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1256040</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2181240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -2952,42 +2838,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4186800" y="5009040"/>
-        <a:ext cx="5760360" cy="3232080"/>
+        <a:off x="186840" y="986400"/>
+        <a:ext cx="5162400" cy="2127960"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>159840</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>62280</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1229400</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>2190600</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame>
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name=""/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="159840" y="995400"/>
-        <a:ext cx="5162760" cy="2128320"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3001,24 +2857,24 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>328320</xdr:colOff>
+      <xdr:colOff>355320</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>30600</xdr:rowOff>
+      <xdr:rowOff>21600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>1994760</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>166320</xdr:rowOff>
+      <xdr:colOff>1056600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2227320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvPr id="4" name=""/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="328320" y="789840"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="355320" y="780840"/>
+        <a:ext cx="4794480" cy="2205720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3036,15 +2892,45 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>349920</xdr:colOff>
+      <xdr:colOff>196560</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>50400</xdr:rowOff>
+      <xdr:rowOff>18720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>619200</xdr:colOff>
+      <xdr:colOff>1862640</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>343440</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name=""/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="196560" y="936720"/>
+        <a:ext cx="5759280" cy="3048840"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1220760</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>2199600</xdr:rowOff>
+      <xdr:rowOff>167400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>4746600</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>2212920</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3052,12 +2938,12 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="349920" y="968400"/>
-        <a:ext cx="4362480" cy="2149200"/>
+        <a:off x="5313960" y="1085400"/>
+        <a:ext cx="3525840" cy="2045520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3071,7 +2957,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G65536"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
@@ -3264,6 +3150,7 @@
       <c r="F20" s="20"/>
     </row>
     <row r="21" customFormat="false" ht="18.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B1:F1"/>
@@ -3295,7 +3182,7 @@
   <dimension ref="A1:U22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3318,7 +3205,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3326,7 +3213,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3339,7 +3226,7 @@
       <c r="A5" s="60"/>
       <c r="B5" s="60"/>
       <c r="C5" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3348,19 +3235,19 @@
       </c>
       <c r="B6" s="48"/>
       <c r="Q6" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="T6" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="U6" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3368,10 +3255,10 @@
         <v>36</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">AVERAGE(R7:U7)</f>
@@ -3392,13 +3279,13 @@
     </row>
     <row r="8" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="P8" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>150</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>140</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">AVERAGE(R8:U8)</f>
@@ -3419,27 +3306,27 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="48"/>
     </row>
     <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B10" s="52"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>26</v>
@@ -3447,32 +3334,32 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="48"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3485,38 +3372,38 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="53"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="61" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B19" s="61"/>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="54" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="55" t="s">
+        <v>153</v>
+      </c>
+      <c r="B21" s="27" t="s">
         <v>154</v>
-      </c>
-      <c r="B21" s="27" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="56" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -3548,8 +3435,8 @@
   </sheetPr>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3572,7 +3459,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3580,7 +3467,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,7 +3480,7 @@
       <c r="A5" s="60"/>
       <c r="B5" s="60"/>
       <c r="C5" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3602,19 +3489,19 @@
       </c>
       <c r="B6" s="48"/>
       <c r="Q6" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="T6" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="U6" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3622,10 +3509,10 @@
         <v>36</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">AVERAGE(R7:U7)</f>
@@ -3646,13 +3533,13 @@
     </row>
     <row r="8" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>159</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">AVERAGE(R8:U8)</f>
@@ -3673,7 +3560,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="48"/>
     </row>
@@ -3685,15 +3572,15 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>26</v>
@@ -3701,32 +3588,32 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="48"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3739,7 +3626,7 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="53"/>
     </row>
@@ -3754,7 +3641,7 @@
         <v>162</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3802,8 +3689,8 @@
   </sheetPr>
   <dimension ref="1:47"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B31" activeCellId="0" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -12051,7 +11938,7 @@
       <c r="AMI8" s="0"/>
       <c r="AMJ8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A9" s="0"/>
       <c r="B9" s="27" t="s">
         <v>40</v>
@@ -13084,9 +12971,7 @@
       <c r="B10" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="18" t="s">
-        <v>42</v>
-      </c>
+      <c r="C10" s="18"/>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
@@ -14112,7 +13997,7 @@
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A11" s="0"/>
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="0"/>
@@ -15140,7 +15025,7 @@
     <row r="12" customFormat="false" ht="115.65" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A12" s="0"/>
       <c r="B12" s="27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="27"/>
       <c r="D12" s="0"/>
@@ -16168,10 +16053,10 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A13" s="0"/>
       <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
@@ -17198,7 +17083,7 @@
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A14" s="0"/>
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>26</v>
@@ -18228,7 +18113,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A15" s="0"/>
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="0"/>
@@ -19256,10 +19141,10 @@
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A16" s="0"/>
       <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="0"/>
@@ -20286,10 +20171,10 @@
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A17" s="0"/>
       <c r="B17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D17" s="0"/>
       <c r="E17" s="0"/>
@@ -21316,10 +21201,10 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="A18" s="0"/>
       <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="D18" s="0"/>
       <c r="E18" s="0"/>
@@ -23376,7 +23261,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="A20" s="0"/>
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="28"/>
       <c r="D20" s="0"/>
@@ -24403,16 +24288,16 @@
     </row>
     <row r="21" s="29" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B21" s="30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="30"/>
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B22" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="32" t="s">
         <v>56</v>
-      </c>
-      <c r="C22" s="32" t="s">
-        <v>57</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -24421,10 +24306,10 @@
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="6" t="s">
         <v>58</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>59</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -24433,10 +24318,10 @@
     </row>
     <row r="24" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="C24" s="8" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>61</v>
       </c>
       <c r="AA24" s="0"/>
       <c r="AB24" s="0"/>
@@ -24523,7 +24408,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA38" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB38" s="22" t="s">
         <v>38</v>
@@ -24532,12 +24417,12 @@
         <v>40</v>
       </c>
       <c r="AD38" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB39" s="22" t="n">
         <v>100</v>
@@ -24552,7 +24437,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB40" s="22" t="n">
         <v>234</v>
@@ -24567,7 +24452,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA41" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB41" s="22" t="n">
         <v>543</v>
@@ -24582,7 +24467,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA42" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB42" s="22" t="n">
         <v>342</v>
@@ -24597,7 +24482,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA43" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB43" s="22" t="n">
         <v>344</v>
@@ -24612,7 +24497,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="22" t="n">
         <v>532</v>
@@ -24627,7 +24512,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA45" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB45" s="22" t="n">
         <v>534</v>
@@ -24657,7 +24542,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB47" s="22" t="n">
         <v>324</v>
@@ -24675,7 +24560,7 @@
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="C8:C9"/>
+    <mergeCell ref="C8:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B15:C15"/>
@@ -24700,7 +24585,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -24733,7 +24618,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -24742,10 +24627,10 @@
     </row>
     <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B3" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>73</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>74</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -24794,19 +24679,17 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>76</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C8" s="18"/>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
       <c r="AC8" s="0"/>
       <c r="AD8" s="0"/>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
+    <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -24819,7 +24702,7 @@
         <v>41</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="AA10" s="0"/>
       <c r="AB10" s="0"/>
@@ -24828,7 +24711,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="14"/>
       <c r="AA11" s="0"/>
@@ -24838,7 +24721,7 @@
     </row>
     <row r="12" customFormat="false" ht="63.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -24848,10 +24731,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="AA13" s="0"/>
       <c r="AB13" s="0"/>
@@ -24860,7 +24743,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>26</v>
@@ -24872,7 +24755,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="14"/>
       <c r="AA15" s="0"/>
@@ -24882,10 +24765,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="AA16" s="0"/>
       <c r="AB16" s="0"/>
@@ -24894,10 +24777,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -24906,10 +24789,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="AA18" s="0"/>
       <c r="AB18" s="0"/>
@@ -24930,7 +24813,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
@@ -24940,10 +24823,10 @@
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B21" s="31" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -24952,10 +24835,10 @@
     </row>
     <row r="22" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="33" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -24964,10 +24847,10 @@
     </row>
     <row r="23" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="34" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -25060,21 +24943,21 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA38" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB38" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="AC38" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="AC38" s="22" t="s">
-        <v>77</v>
-      </c>
       <c r="AD38" s="22" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB39" s="36" t="n">
         <v>3287</v>
@@ -25089,7 +24972,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB40" s="36" t="n">
         <v>5344</v>
@@ -25104,7 +24987,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA41" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB41" s="36" t="n">
         <v>3423</v>
@@ -25119,7 +25002,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA42" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB42" s="36" t="n">
         <v>40000</v>
@@ -25134,7 +25017,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA43" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB43" s="36" t="n">
         <v>5467</v>
@@ -25149,7 +25032,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="36" t="n">
         <v>532</v>
@@ -25164,7 +25047,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA45" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB45" s="36" t="n">
         <v>534</v>
@@ -25194,7 +25077,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB47" s="36" t="n">
         <v>324</v>
@@ -25236,7 +25119,7 @@
   <dimension ref="B1:AD47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25269,7 +25152,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -25281,7 +25164,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -25330,10 +25213,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -25342,7 +25225,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -25352,7 +25235,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="18"/>
       <c r="AA10" s="0"/>
@@ -25362,7 +25245,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="14"/>
       <c r="AA11" s="0"/>
@@ -25372,7 +25255,7 @@
     </row>
     <row r="12" customFormat="false" ht="37.5" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -25382,10 +25265,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="AA13" s="0"/>
       <c r="AB13" s="0"/>
@@ -25394,7 +25277,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>26</v>
@@ -25406,7 +25289,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="14"/>
       <c r="AA15" s="0"/>
@@ -25416,10 +25299,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="AA16" s="0"/>
       <c r="AB16" s="0"/>
@@ -25428,10 +25311,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -25440,10 +25323,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="AA18" s="0"/>
       <c r="AB18" s="0"/>
@@ -25464,7 +25347,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
@@ -25474,10 +25357,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B21" s="39" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" s="40" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -25486,10 +25369,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -25498,10 +25381,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -25594,7 +25477,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA38" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB38" s="22" t="s">
         <v>38</v>
@@ -25603,12 +25486,12 @@
         <v>40</v>
       </c>
       <c r="AD38" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB39" s="22" t="n">
         <v>100</v>
@@ -25623,7 +25506,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB40" s="22" t="n">
         <v>234</v>
@@ -25638,7 +25521,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA41" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB41" s="22" t="n">
         <v>543</v>
@@ -25653,7 +25536,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA42" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB42" s="22" t="n">
         <v>342</v>
@@ -25668,7 +25551,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA43" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB43" s="22" t="n">
         <v>344</v>
@@ -25683,7 +25566,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="22" t="n">
         <v>532</v>
@@ -25698,7 +25581,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA45" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB45" s="22" t="n">
         <v>534</v>
@@ -25728,7 +25611,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB47" s="22" t="n">
         <v>324</v>
@@ -25803,7 +25686,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -25815,7 +25698,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -25864,10 +25747,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -25876,7 +25759,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="43"/>
       <c r="AA9" s="0"/>
@@ -25886,7 +25769,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="43"/>
       <c r="AA10" s="0"/>
@@ -25896,7 +25779,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="14"/>
       <c r="AA11" s="0"/>
@@ -25906,7 +25789,7 @@
     </row>
     <row r="12" customFormat="false" ht="39.75" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -25916,10 +25799,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="AA13" s="0"/>
       <c r="AB13" s="0"/>
@@ -25928,7 +25811,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>26</v>
@@ -25940,7 +25823,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="14"/>
       <c r="AA15" s="0"/>
@@ -25950,10 +25833,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="AA16" s="0"/>
       <c r="AB16" s="0"/>
@@ -25962,10 +25845,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -25974,10 +25857,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="AA18" s="0"/>
       <c r="AB18" s="0"/>
@@ -25998,7 +25881,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
@@ -26008,10 +25891,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B21" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -26020,10 +25903,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -26032,10 +25915,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -26128,7 +26011,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA38" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB38" s="22" t="s">
         <v>38</v>
@@ -26137,12 +26020,12 @@
         <v>40</v>
       </c>
       <c r="AD38" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB39" s="22" t="n">
         <v>100</v>
@@ -26157,7 +26040,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB40" s="22" t="n">
         <v>234</v>
@@ -26172,7 +26055,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA41" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB41" s="22" t="n">
         <v>543</v>
@@ -26187,7 +26070,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA42" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB42" s="22" t="n">
         <v>342</v>
@@ -26202,7 +26085,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA43" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB43" s="22" t="n">
         <v>344</v>
@@ -26217,7 +26100,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="22" t="n">
         <v>532</v>
@@ -26232,7 +26115,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA45" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB45" s="22" t="n">
         <v>534</v>
@@ -26262,7 +26145,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB47" s="22" t="n">
         <v>324</v>
@@ -26337,7 +26220,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -26349,7 +26232,7 @@
         <v>32</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -26398,10 +26281,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -26410,7 +26293,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -26420,7 +26303,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="18"/>
       <c r="AA10" s="0"/>
@@ -26430,7 +26313,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="14"/>
       <c r="AA11" s="0"/>
@@ -26440,7 +26323,7 @@
     </row>
     <row r="12" customFormat="false" ht="46.9" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -26450,10 +26333,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="AA13" s="0"/>
       <c r="AB13" s="0"/>
@@ -26462,7 +26345,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>26</v>
@@ -26474,7 +26357,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="14"/>
       <c r="AA15" s="0"/>
@@ -26484,10 +26367,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="AA16" s="0"/>
       <c r="AB16" s="0"/>
@@ -26496,10 +26379,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -26508,10 +26391,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="AA18" s="0"/>
       <c r="AB18" s="0"/>
@@ -26532,7 +26415,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
@@ -26542,10 +26425,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B21" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -26554,10 +26437,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -26566,10 +26449,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -26662,7 +26545,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA38" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB38" s="22" t="s">
         <v>38</v>
@@ -26671,12 +26554,12 @@
         <v>40</v>
       </c>
       <c r="AD38" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB39" s="22" t="n">
         <v>100</v>
@@ -26691,7 +26574,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB40" s="22" t="n">
         <v>234</v>
@@ -26706,7 +26589,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA41" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB41" s="22" t="n">
         <v>543</v>
@@ -26721,7 +26604,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA42" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB42" s="22" t="n">
         <v>342</v>
@@ -26736,7 +26619,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA43" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB43" s="22" t="n">
         <v>344</v>
@@ -26751,7 +26634,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="22" t="n">
         <v>532</v>
@@ -26766,7 +26649,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA45" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB45" s="22" t="n">
         <v>534</v>
@@ -26796,7 +26679,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB47" s="22" t="n">
         <v>324</v>
@@ -26871,7 +26754,7 @@
         <v>30</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AA2" s="0"/>
       <c r="AB2" s="0"/>
@@ -26880,10 +26763,10 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B3" s="23" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AA3" s="0"/>
       <c r="AB3" s="0"/>
@@ -26932,10 +26815,10 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B8" s="27" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C8" s="18" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AA8" s="0"/>
       <c r="AB8" s="0"/>
@@ -26944,7 +26827,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B9" s="27" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C9" s="18"/>
       <c r="AA9" s="0"/>
@@ -26954,7 +26837,7 @@
     </row>
     <row r="10" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B10" s="27" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C10" s="18"/>
       <c r="AA10" s="0"/>
@@ -26964,7 +26847,7 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B11" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="14"/>
       <c r="AA11" s="0"/>
@@ -26974,7 +26857,7 @@
     </row>
     <row r="12" customFormat="false" ht="45.6" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B12" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C12" s="27"/>
       <c r="AA12" s="0"/>
@@ -26984,10 +26867,10 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B13" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>45</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>46</v>
       </c>
       <c r="AA13" s="0"/>
       <c r="AB13" s="0"/>
@@ -26996,7 +26879,7 @@
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>26</v>
@@ -27008,7 +26891,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B15" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="14"/>
       <c r="AA15" s="0"/>
@@ -27018,10 +26901,10 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B16" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="14" t="s">
         <v>49</v>
-      </c>
-      <c r="C16" s="14" t="s">
-        <v>50</v>
       </c>
       <c r="AA16" s="0"/>
       <c r="AB16" s="0"/>
@@ -27030,10 +26913,10 @@
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C17" s="17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="AA17" s="0"/>
       <c r="AB17" s="0"/>
@@ -27042,10 +26925,10 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B18" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="14" t="s">
         <v>52</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>53</v>
       </c>
       <c r="AA18" s="0"/>
       <c r="AB18" s="0"/>
@@ -27066,7 +26949,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="1" collapsed="false">
       <c r="B20" s="28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C20" s="28"/>
       <c r="AA20" s="0"/>
@@ -27076,10 +26959,10 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="1" collapsed="false">
       <c r="B21" s="44" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C21" s="32" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="AA21" s="0"/>
       <c r="AB21" s="0"/>
@@ -27088,10 +26971,10 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="41" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="AA22" s="0"/>
       <c r="AB22" s="0"/>
@@ -27100,10 +26983,10 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="42" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="AA23" s="0"/>
       <c r="AB23" s="0"/>
@@ -27196,7 +27079,7 @@
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA38" s="22" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AB38" s="22" t="s">
         <v>38</v>
@@ -27205,12 +27088,12 @@
         <v>40</v>
       </c>
       <c r="AD38" s="22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA39" s="22" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AB39" s="22" t="n">
         <v>100</v>
@@ -27225,7 +27108,7 @@
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA40" s="22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="AB40" s="22" t="n">
         <v>234</v>
@@ -27240,7 +27123,7 @@
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA41" s="22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="AB41" s="22" t="n">
         <v>543</v>
@@ -27255,7 +27138,7 @@
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA42" s="22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="AB42" s="22" t="n">
         <v>342</v>
@@ -27270,7 +27153,7 @@
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA43" s="22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="AB43" s="22" t="n">
         <v>344</v>
@@ -27285,7 +27168,7 @@
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA44" s="22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB44" s="22" t="n">
         <v>532</v>
@@ -27300,7 +27183,7 @@
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA45" s="22" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="AB45" s="22" t="n">
         <v>534</v>
@@ -27330,7 +27213,7 @@
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="AA47" s="22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="AB47" s="22" t="n">
         <v>324</v>
@@ -27373,7 +27256,7 @@
   <dimension ref="A1:B23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27396,7 +27279,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27404,7 +27287,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27428,52 +27311,52 @@
         <v>36</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="50" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B8" s="51" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="50" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B9" s="51"/>
     </row>
     <row r="10" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="27" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="51"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="48"/>
     </row>
     <row r="12" customFormat="false" ht="45.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="52" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B12" s="52"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="48" t="s">
         <v>45</v>
-      </c>
-      <c r="B13" s="48" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B14" s="27" t="s">
         <v>26</v>
@@ -27481,32 +27364,32 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B15" s="48"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B16" s="48" t="s">
         <v>49</v>
-      </c>
-      <c r="B16" s="48" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B18" s="48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27519,32 +27402,32 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20" s="53"/>
     </row>
     <row r="21" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="54" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="55" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="56" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B23" s="27" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -27576,8 +27459,8 @@
   </sheetPr>
   <dimension ref="A1:U22"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -27601,7 +27484,7 @@
         <v>30</v>
       </c>
       <c r="B2" s="47" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27609,7 +27492,7 @@
         <v>32</v>
       </c>
       <c r="B3" s="47" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27620,11 +27503,11 @@
     </row>
     <row r="5" customFormat="false" ht="184.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="60" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B5" s="60"/>
       <c r="C5" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -27633,19 +27516,19 @@
       </c>
       <c r="B6" s="48"/>
       <c r="Q6" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="R6" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="S6" s="0" t="s">
         <v>132</v>
       </c>
-      <c r="R6" s="0" t="s">
+      <c r="T6" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="S6" s="0" t="s">
+      <c r="U6" s="0" t="s">
         <v>134</v>
-      </c>
-      <c r="T6" s="0" t="s">
-        <v>135</v>
-      </c>
-      <c r="U6" s="0" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27653,10 +27536,10 @@
         <v>36</v>
       </c>
       <c r="B7" s="48" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="Q7" s="0" t="n">
         <f aca="false">AVERAGE(R7:U7)</f>
@@ -27677,13 +27560,13 @@
     </row>
     <row r="8" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="27" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="P8" s="0" t="s">
         <v>138</v>
-      </c>
-      <c r="B8" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="P8" s="0" t="s">
-        <v>140</v>
       </c>
       <c r="Q8" s="0" t="n">
         <f aca="false">AVERAGE(R8:U8)</f>
@@ -27704,27 +27587,27 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B9" s="48"/>
     </row>
     <row r="10" customFormat="false" ht="61.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="52" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B10" s="52"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="48" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="48" t="s">
         <v>45</v>
-      </c>
-      <c r="B11" s="48" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>26</v>
@@ -27732,32 +27615,32 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13" s="48"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="48" t="s">
         <v>49</v>
-      </c>
-      <c r="B14" s="48" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B15" s="27" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="48" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B16" s="48" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27770,38 +27653,38 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="53" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B18" s="53"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="61" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B19" s="61"/>
     </row>
     <row r="20" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="54" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B20" s="27" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="55" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B21" s="27" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="56" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B22" s="27" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>

</xml_diff>